<commit_message>
Refactor database schema and improve property processing logic
Revised database schema to simplify structure, added default values to multiple columns, and ensured foreign key relationships are properly set. Enhanced property processing functionalities, introducing dynamic truncation and automated description generation. Updated price processing to enforce logical constraints on minimum offer and auto-accept prices.
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\PycharmProjects\booklookerBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FD6C88-71DD-4D0B-BA94-7EAF0F77FF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818B292C-BA49-433D-A687-05D55744D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="10668" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>https://www.booklooker.de/B%C3%BCcher/Kapverden/us/2482</t>
+    <t>https://www.booklooker.de/B%C3%BCcher/Angebote/sparteID=581&amp;searchUserTyp=2&amp;zustand=2&amp;paymentMethods%5B6%5D=1?sortOrder=preis_total</t>
   </si>
 </sst>
 </file>
@@ -347,9 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>